<commit_message>
update at 2018-9-29 12:28:10
</commit_message>
<xml_diff>
--- a/第10组/项目计划表.xlsx
+++ b/第10组/项目计划表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>日期：2018.9.29 第五周周四</t>
   </si>
@@ -76,6 +76,14 @@
   </si>
   <si>
     <t>查看需求分析，分析&lt;定位&gt;功能模块</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>总结：已进行项目需求分析讨论，并通过分析确定每个功能模块的功能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂时未得知如何设计用例图</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -143,7 +151,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -151,6 +159,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -463,7 +474,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -474,12 +485,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -502,7 +513,9 @@
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -512,7 +525,9 @@
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -522,7 +537,9 @@
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -532,7 +549,9 @@
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -542,30 +561,34 @@
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
@@ -612,18 +635,18 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>